<commit_message>
17MAY data pull and analysis
</commit_message>
<xml_diff>
--- a/Results/Sources.xlsx
+++ b/Results/Sources.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25240" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18620" windowHeight="16640" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Source Results" sheetId="2" r:id="rId1"/>
+    <sheet name="Sources_17May" sheetId="3" r:id="rId1"/>
+    <sheet name="Sources_16May" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>CNN</t>
   </si>
@@ -510,13 +511,19 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -550,6 +557,335 @@
         <v>9</v>
       </c>
       <c r="B2">
+        <v>37</v>
+      </c>
+      <c r="C2">
+        <v>75.7</v>
+      </c>
+      <c r="D2">
+        <v>24.3</v>
+      </c>
+      <c r="E2">
+        <f>C2-D2</f>
+        <v>51.400000000000006</v>
+      </c>
+      <c r="F2">
+        <f>AVERAGE(E2:E13)</f>
+        <v>57.366666666666674</v>
+      </c>
+      <c r="G2">
+        <f>STDEV(E2:E13)</f>
+        <v>38.020743939288842</v>
+      </c>
+      <c r="H2">
+        <f>(E2-$F$2)/$G$2</f>
+        <v>-0.15693187582531748</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>151</v>
+      </c>
+      <c r="C3">
+        <v>93.4</v>
+      </c>
+      <c r="D3">
+        <v>6.6</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E13" si="0">C3-D3</f>
+        <v>86.800000000000011</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H13" si="1">(E3-$F$2)/$G$2</f>
+        <v>0.77413880644556032</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>173</v>
+      </c>
+      <c r="C4">
+        <v>84.4</v>
+      </c>
+      <c r="D4">
+        <v>15.6</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>68.800000000000011</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>0.30071303579935138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>92.6</v>
+      </c>
+      <c r="D5">
+        <v>7.4</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>85.199999999999989</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0.73205651572145225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>83.3</v>
+      </c>
+      <c r="D6">
+        <v>16.7</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>66.599999999999994</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>0.24284988605370317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>94</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0.80570052448864071</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>61</v>
+      </c>
+      <c r="C8">
+        <v>45.9</v>
+      </c>
+      <c r="D8">
+        <v>54.1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>-8.2000000000000028</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>-1.7244972052983207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>71</v>
+      </c>
+      <c r="C9">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="D9">
+        <v>21.1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>57.800000000000004</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1.1397287071112351E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <v>93.5</v>
+      </c>
+      <c r="D10">
+        <v>6.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>0.77939909278607356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>85.2</v>
+      </c>
+      <c r="D11">
+        <v>14.8</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0.34279532652345868</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>83</v>
+      </c>
+      <c r="C12">
+        <v>34.9</v>
+      </c>
+      <c r="D12">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>-30.199999999999996</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>-2.303128702754798</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>51</v>
+      </c>
+      <c r="C13">
+        <v>82.4</v>
+      </c>
+      <c r="D13">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>64.800000000000011</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0.1955073089890827</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
         <v>31</v>
       </c>
       <c r="C2" s="1">
@@ -563,16 +899,16 @@
         <v>48.400000000000006</v>
       </c>
       <c r="F2" s="1">
-        <f>AVERAGE($E2:E13)</f>
-        <v>63.20000000000001</v>
-      </c>
-      <c r="G2">
-        <f>STDEV(E2:E13)</f>
-        <v>36.837925121710178</v>
-      </c>
-      <c r="H2">
+        <f>AVERAGE($E2:E2)</f>
+        <v>48.400000000000006</v>
+      </c>
+      <c r="G2" t="e">
+        <f>STDEV(E2:E2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H2" t="e">
         <f>(E2-$F$2)/$G$2</f>
-        <v>-0.40175986978370087</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -588,15 +924,6 @@
       <c r="D3" s="1">
         <v>1.4</v>
       </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E13" si="0">C3-D3</f>
-        <v>97.199999999999989</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="H3">
-        <f t="shared" ref="H3:H13" si="1">(E3-$F$2)/$G$2</f>
-        <v>0.92296186301660932</v>
-      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
@@ -611,15 +938,6 @@
       <c r="D4" s="1">
         <v>13.8</v>
       </c>
-      <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>72.400000000000006</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>0.2497426217574355</v>
-      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
@@ -634,15 +952,6 @@
       <c r="D5" s="1">
         <v>7.4</v>
       </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>85.199999999999989</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>0.59721061724604108</v>
-      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
@@ -657,15 +966,6 @@
       <c r="D6" s="1">
         <v>17.5</v>
       </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>4.886268686558496E-2</v>
-      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -680,15 +980,6 @@
       <c r="D7" s="1">
         <v>7.5</v>
       </c>
-      <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>0.59178142981653192</v>
-      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -703,15 +994,6 @@
       <c r="D8" s="1">
         <v>55</v>
       </c>
-      <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>-10</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>-1.9870825992004664</v>
-      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -726,15 +1008,6 @@
       <c r="D9" s="1">
         <v>23</v>
       </c>
-      <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>-0.24974262175743586</v>
-      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
@@ -749,15 +1022,6 @@
       <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E10" s="1">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="H10">
-        <f t="shared" si="1"/>
-        <v>0.99897048702974212</v>
-      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
@@ -772,15 +1036,6 @@
       <c r="D11" s="1">
         <v>11.5</v>
       </c>
-      <c r="E11" s="1">
-        <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="H11">
-        <f t="shared" si="1"/>
-        <v>0.37461393263615311</v>
-      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -795,15 +1050,6 @@
       <c r="D12" s="1">
         <v>53</v>
       </c>
-      <c r="E12" s="1">
-        <f t="shared" si="0"/>
-        <v>-6</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="H12">
-        <f t="shared" si="1"/>
-        <v>-1.8784988506102769</v>
-      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -817,15 +1063,6 @@
       </c>
       <c r="D13" s="1">
         <v>4.9000000000000004</v>
-      </c>
-      <c r="E13" s="1">
-        <f t="shared" si="0"/>
-        <v>90.199999999999989</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="H13">
-        <f t="shared" si="1"/>
-        <v>0.73294030298377788</v>
       </c>
     </row>
   </sheetData>

</xml_diff>